<commit_message>
More improvement added to code.
</commit_message>
<xml_diff>
--- a/2023-10-01Sales.xlsx
+++ b/2023-10-01Sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>PC</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>5400</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>4000</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -707,6 +716,86 @@
         <v>31</v>
       </c>
     </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>